<commit_message>
Added image - animatronic
</commit_message>
<xml_diff>
--- a/scripts/projects.xlsx
+++ b/scripts/projects.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pp_portfolio_website\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/the_seeker_soul/Desktop/panktiparekh15.github.io/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179A4B28-934D-4735-89D3-477AA7685338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BEF8CB-3BFD-4144-ADE9-40FAF556A086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{602863E7-E81E-D041-B2B4-436E4560BFF8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{602863E7-E81E-D041-B2B4-436E4560BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>proj_name</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>target-selection-for-mergers-acquisitions</t>
+  </si>
+  <si>
+    <t>assets/animatronic-hand.png</t>
   </si>
 </sst>
 </file>
@@ -668,26 +671,26 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.19921875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="6" customWidth="1"/>
     <col min="5" max="6" width="35.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="150.69921875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="150.6640625" style="5" customWidth="1"/>
     <col min="8" max="15" width="35.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.796875" style="1"/>
+    <col min="16" max="16" width="10.83203125" style="1"/>
     <col min="17" max="17" width="48" style="1" customWidth="1"/>
     <col min="18" max="18" width="55" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.796875" style="1"/>
-    <col min="20" max="16384" width="10.796875" style="2"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -733,7 +736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -756,7 +759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -779,7 +782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -802,7 +805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -825,7 +828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -848,7 +851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -871,7 +874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -885,7 +888,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>4</v>
@@ -894,11 +897,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D57" s="7"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -912,10 +915,10 @@
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="5"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
     </row>

</xml_diff>

<commit_message>
separated banner image and thumbnail image
</commit_message>
<xml_diff>
--- a/scripts/projects.xlsx
+++ b/scripts/projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/the_seeker_soul/Desktop/panktiparekh15.github.io/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\panktiparekh15.github.io\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884A2C1D-9D18-BA45-AA06-A0C958F8BC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E7CE6-2B50-4E4A-B46E-5B7C38E8EDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{602863E7-E81E-D041-B2B4-436E4560BFF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{602863E7-E81E-D041-B2B4-436E4560BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>proj_name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>project_date</t>
   </si>
   <si>
-    <t>project_img</t>
-  </si>
-  <si>
     <t>Deep Image Colorization using Transfer Learning</t>
   </si>
   <si>
@@ -99,51 +96,6 @@
     <t>assets/video-keyframe.jpg</t>
   </si>
   <si>
-    <t>&lt;p&gt;Utilized K-means clustering to group images with identical semantic&lt;/p&gt;
-composition and reconstructed keyframe from cluste centers.
-Used YOLOv3 to compare the performance on both the original and the summarised versions of the video to evaluate accuracy of the algorithm.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Hello, I am Pankti Parekh.&lt;/p&gt;
-&lt;pre&gt;
-&lt;code class="language-cpp"&gt;&amp;lt;section class="section__copyright bg--dark"&amp;gt;
-	&amp;lt;div class="container"&amp;gt;
-		&amp;lt;div class="row"&amp;gt;
-			&amp;lt;div class="col-md-12 text-center"&amp;gt;
-				&amp;lt;p class="heading mb-4"&amp;gt;© 2022. All Rights Reserved.&amp;lt;/p&amp;gt;
-				&amp;lt;p class="credit"&amp;gt;Designed &amp;amp; Developed by &amp;lt;a href="" class="text--lightp"&amp;gt;Jahanvi Jasani&amp;lt;/a&amp;gt;&amp;lt;/p&amp;gt;
-			&amp;lt;/div&amp;gt;
-		&amp;lt;/div&amp;gt;
-	&amp;lt;/div&amp;gt;
-&amp;lt;/section&amp;gt;&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;pre class="hljs" style="display: block; overflow-x: auto; background: rgb(0, 36, 81); color: rgb(255, 255, 255); padding: 0.5em;"&gt;&amp;lt;section &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"section__copyright bg--dark"&lt;/span&gt;&amp;gt;
-	&amp;lt;div &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"container"&lt;/span&gt;&amp;gt;
-		&amp;lt;div &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"row"&lt;/span&gt;&amp;gt;
-			&amp;lt;div &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"col-md-12 text-center"&lt;/span&gt;&amp;gt;
-				&amp;lt;p &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"heading mb-4"&lt;/span&gt;&amp;gt;© &lt;span class="hljs-number" style="color: rgb(255, 197, 143);"&gt;2022.&lt;/span&gt; All Rights Reserved.&amp;lt;/p&amp;gt;
-				&amp;lt;p &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"credit"&lt;/span&gt;&amp;gt;Designed &amp;amp; Developed by &amp;lt;a href=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;""&lt;/span&gt; &lt;span class="hljs-keyword" style="color: rgb(235, 187, 255);"&gt;class&lt;/span&gt;=&lt;span class="hljs-string" style="color: rgb(209, 241, 169);"&gt;"text--lightp"&lt;/span&gt;&amp;gt;Jahanvi Jasani&amp;lt;/a&amp;gt;&amp;lt;/p&amp;gt;
-			&amp;lt;/div&amp;gt;
-		&amp;lt;/div&amp;gt;
-	&amp;lt;/div&amp;gt;
-&amp;lt;/section&amp;gt;&lt;/pre&gt;</t>
-  </si>
-  <si>
-    <t>&lt;pre&gt;
-&amp;lt;section &lt;span style="color:#ebbbff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;section__copyright&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;bg&lt;/span&gt;--&lt;span style="color:#bbdaff"&gt;dark&lt;/span&gt;&amp;quot;&amp;gt;
-   &amp;lt;&lt;span style="color:#bbdaff"&gt;div&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;container&lt;/span&gt;&amp;quot;&amp;gt;
-      &amp;lt;&lt;span style="color:#bbdaff"&gt;div&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;row&lt;/span&gt;&amp;quot;&amp;gt;
-         &amp;lt;&lt;span style="color:#bbdaff"&gt;div&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;col&lt;/span&gt;-&lt;span style="color:#bbdaff"&gt;md&lt;/span&gt;-12 &lt;span style="color:#bbdaff"&gt;text&lt;/span&gt;-&lt;span style="color:#bbdaff"&gt;center&lt;/span&gt;&amp;quot;&amp;gt;
-            &amp;lt;&lt;span style="color:#bbdaff"&gt;p&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;heading&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;mb&lt;/span&gt;-4&amp;quot;&amp;gt;&amp;copy; 2022. &lt;span style="color:#bbdaff"&gt;All&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;Rights&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;Reserved&lt;/span&gt;.&amp;lt;/&lt;span style="color:#bbdaff"&gt;p&lt;/span&gt;&amp;gt;
-            &amp;lt;&lt;span style="color:#bbdaff"&gt;p&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;credit&lt;/span&gt;&amp;quot;&amp;gt;&lt;span style="color:#bbdaff"&gt;Designed&lt;/span&gt; &amp;amp; &lt;span style="color:#bbdaff"&gt;Developed&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;by&lt;/span&gt; &amp;lt;&lt;span style="color:#bbdaff"&gt;a&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;href&lt;/span&gt;=&amp;quot;&amp;quot; &lt;span style="color:#bbdaff"&gt;class&lt;/span&gt;=&amp;quot;&lt;span style="color:#bbdaff"&gt;text&lt;/span&gt;--&lt;span style="color:#bbdaff"&gt;lightp&lt;/span&gt;&amp;quot;&amp;gt;&lt;span style="color:#bbdaff"&gt;Jahanvi&lt;/span&gt; &lt;span style="color:#bbdaff"&gt;Jasani&lt;/span&gt;&amp;lt;/&lt;span style="color:#bbdaff"&gt;a&lt;/span&gt;&amp;gt;&amp;lt;/&lt;span style="color:#bbdaff"&gt;p&lt;/span&gt;&amp;gt;
-         &amp;lt;/&lt;span style="color:#bbdaff"&gt;div&lt;/span&gt;&amp;gt;
-      &amp;lt;/&lt;span style="color:#bbdaff"&gt;div&lt;/span&gt;&amp;gt;
-   &amp;lt;/&lt;span style="color:#bbdaff"&gt;div&lt;/span&gt;&amp;gt;
-&amp;lt;/&lt;span style="color:#bbdaff"&gt;section&lt;/span&gt;&amp;gt;&lt;/pre&gt;</t>
-  </si>
-  <si>
     <t>glaucoma-detection</t>
   </si>
   <si>
@@ -184,6 +136,12 @@
   </si>
   <si>
     <t>assets/stitch.png</t>
+  </si>
+  <si>
+    <t>thumbnail_img</t>
+  </si>
+  <si>
+    <t>banner_img</t>
   </si>
 </sst>
 </file>
@@ -682,35 +640,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A650391-D44E-E944-A89C-DDEE829408A0}">
-  <dimension ref="A1:S155"/>
+  <dimension ref="A1:T155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="6" customWidth="1"/>
-    <col min="5" max="6" width="35.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="150.6640625" style="5" customWidth="1"/>
-    <col min="8" max="15" width="35.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="48" style="1" customWidth="1"/>
-    <col min="18" max="18" width="55" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="33.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" style="6" customWidth="1"/>
+    <col min="5" max="7" width="35.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="150.69921875" style="5" customWidth="1"/>
+    <col min="9" max="16" width="35.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.796875" style="1"/>
+    <col min="18" max="18" width="48" style="1" customWidth="1"/>
+    <col min="19" max="19" width="55" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.796875" style="1"/>
+    <col min="21" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -719,204 +677,207 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="36" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="40" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="36" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="36" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="36" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D57" s="7"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -929,16 +890,17 @@
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="P57" s="4"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="5"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R161">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S161">
     <sortCondition ref="A1:A161"/>
   </sortState>
   <conditionalFormatting sqref="A9:B1048576 A1:B1 A3:A8">
@@ -969,7 +931,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576" xr:uid="{595D32B6-7079-2B4F-892C-5B88B245F55E}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576" xr:uid="{595D32B6-7079-2B4F-892C-5B88B245F55E}">
       <formula1>"easy, medium, hard"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>